<commit_message>
XGL permissions initial commit
</commit_message>
<xml_diff>
--- a/testdata/DBI.xlsx
+++ b/testdata/DBI.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="DBI" sheetId="3" r:id="rId1"/>
+    <sheet name="MCC" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="18">
   <si>
     <t>Category</t>
   </si>
@@ -37,34 +38,34 @@
     <t>Y</t>
   </si>
   <si>
+    <t>Pre-Billing Processing</t>
+  </si>
+  <si>
+    <t>Undo Ad Unit Movement</t>
+  </si>
+  <si>
+    <t>Run Discrepency Analyzer Tool (DAT)</t>
+  </si>
+  <si>
+    <t>View Monthly Pre-Billing</t>
+  </si>
+  <si>
+    <t>View Moved Ad Units Detail</t>
+  </si>
+  <si>
+    <t>View Moved Ad Units List</t>
+  </si>
+  <si>
+    <t>Reconciliation</t>
+  </si>
+  <si>
+    <t>Reconciliation Pre-Billing Processing</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Pre-Billing Processing</t>
-  </si>
-  <si>
-    <t>Undo Ad Unit Movement</t>
-  </si>
-  <si>
-    <t>Run Discrepency Analyzer Tool (DAT)</t>
-  </si>
-  <si>
-    <t>View Monthly Pre-Billing</t>
-  </si>
-  <si>
-    <t>View Moved Ad Units Detail</t>
-  </si>
-  <si>
-    <t>View Moved Ad Units List</t>
-  </si>
-  <si>
-    <t>Reconciliation</t>
-  </si>
-  <si>
-    <t>Reconciliation Pre-Billing Processing</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>Fail</t>
@@ -75,10 +76,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -95,9 +96,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -105,22 +113,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -195,6 +188,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -202,15 +203,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -218,7 +219,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -240,31 +241,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,151 +403,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -434,37 +435,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.399975585192419"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,17 +507,28 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -543,10 +544,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -556,55 +554,58 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -931,7 +932,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -954,7 +955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -965,91 +966,203 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="22.0"/>
+    <col min="2" max="2" customWidth="true" width="37.0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>